<commit_message>
added RMA and conclusion sections to write up for scheduling assignment
</commit_message>
<xml_diff>
--- a/lab_5_c_files/scheduler_comparisons.xlsx
+++ b/lab_5_c_files/scheduler_comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nate\UtahState\USUSpring2024\Embedded_Real-Time_Systems_5780\Assignments\Labs_Reports\lab_5_c_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62470BE6-9CA8-482E-83A7-71E1E87B2DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E239F68-A899-44D3-97BC-E29B031F70AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="11415" windowHeight="14362" xr2:uid="{5E47B806-9857-484F-8AD1-57AAB6BC4C39}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5E47B806-9857-484F-8AD1-57AAB6BC4C39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,14 +127,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -473,47 +472,48 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.73046875" customWidth="1"/>
-    <col min="2" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.53125" customWidth="1"/>
-    <col min="6" max="6" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>0.96</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2">
         <v>600</v>
       </c>
       <c r="D2">
@@ -530,13 +530,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>0.96</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3">
         <v>600</v>
       </c>
       <c r="D3">
@@ -553,13 +553,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>0.96</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>600</v>
       </c>
       <c r="D4">
@@ -576,13 +576,13 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>1.2829999999999999</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>1000</v>
       </c>
       <c r="D5">
@@ -599,13 +599,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>1.2829999999999999</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>1000</v>
       </c>
       <c r="D6">
@@ -622,13 +622,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>1.2829999999999999</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>1000</v>
       </c>
       <c r="D7">
@@ -645,13 +645,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>0.98799999999999999</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8">
         <v>700</v>
       </c>
       <c r="D8">
@@ -668,13 +668,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>0.98799999999999999</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>700</v>
       </c>
       <c r="D9">
@@ -691,13 +691,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>0.98799999999999999</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>700</v>
       </c>
       <c r="D10">

</xml_diff>